<commit_message>
Working updated relationship with bob
</commit_message>
<xml_diff>
--- a/Traits.xlsx
+++ b/Traits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skyler\.GitHub\PrettyBoySims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1493D3EA-DA4A-422E-B85B-6A56B4D77E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3D1291-FA98-4FB1-9714-C7E3DB5F0506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="14596" windowHeight="8476" activeTab="1" xr2:uid="{C91ABEC4-7EDA-4038-8786-2CC169CFE2BD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{C91ABEC4-7EDA-4038-8786-2CC169CFE2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" r:id="rId1"/>
@@ -4067,12 +4067,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4103,13 +4104,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4349,23 +4349,23 @@
     <tableColumn id="2" xr3:uid="{A4B504C6-3BAA-4385-ABE4-300463C9C712}" name="Me" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{4FEA053F-4632-4875-A48C-36EB177BEE56}" name="My" dataDxfId="10"/>
     <tableColumn id="9" xr3:uid="{B9E2DF82-126D-4F8F-8BD1-6EC09F0DABFB}" name="MyPlayed" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{BFB7D7CF-F5D1-493F-AD7F-F187881812ED}" name="Curated" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{7B475C5F-4BC6-458B-A862-3EB6160E968F}" name="Royal" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{6B91F3FC-7871-4680-903E-323C827E44FC}" name="Maid" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{352AA68C-83E0-4F72-A066-4B84946B1285}" name="Nanny" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{1C920CF9-0736-4582-8ADC-DEE92E3CD5B4}" name="Service" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{7C948067-EB35-42B1-9558-2CDBBA457CEC}" name="Slave" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{78FD4BD5-DAB0-492F-B21D-886DE7FFDEC0}" name="Hot" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{BFB7D7CF-F5D1-493F-AD7F-F187881812ED}" name="Curated" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{7B475C5F-4BC6-458B-A862-3EB6160E968F}" name="Royal" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{6B91F3FC-7871-4680-903E-323C827E44FC}" name="Maid" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{352AA68C-83E0-4F72-A066-4B84946B1285}" name="Nanny" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{1C920CF9-0736-4582-8ADC-DEE92E3CD5B4}" name="Service" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{7C948067-EB35-42B1-9558-2CDBBA457CEC}" name="Slave" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{78FD4BD5-DAB0-492F-B21D-886DE7FFDEC0}" name="Hot" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8E158FA-B3F2-41F5-9DEC-7D3D81E08E95}" name="Table1" displayName="Table1" ref="A1:K79" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8E158FA-B3F2-41F5-9DEC-7D3D81E08E95}" name="Table1" displayName="Table1" ref="A1:K79" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:K79" xr:uid="{D8E158FA-B3F2-41F5-9DEC-7D3D81E08E95}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E3223379-F960-4155-A282-89AD61904B22}" name="Skill" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E3223379-F960-4155-A282-89AD61904B22}" name="Skill" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{ACC85313-7EE2-4777-85A6-78CB6646648D}" name="Me"/>
     <tableColumn id="3" xr3:uid="{C71992C7-373A-4B80-B9A3-9DADE757B8B6}" name="My"/>
     <tableColumn id="12" xr3:uid="{BB9FF5FB-6F0E-4BED-968F-6CA93AB99900}" name="MyPlayed"/>
@@ -4700,14 +4700,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3772FFB-52EB-42EA-A7F0-DFC1296DBB8F}">
   <dimension ref="A1:K1180"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1104" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="85.6640625" customWidth="1"/>
+    <col min="1" max="1" width="101.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="6" width="16.796875" customWidth="1"/>
     <col min="7" max="7" width="14.265625" customWidth="1"/>
@@ -41537,7 +41537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47091772-5CAA-4B97-9B7E-07B56B4E4620}">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F74" sqref="F71:F74"/>
     </sheetView>
   </sheetViews>

</xml_diff>